<commit_message>
Arquivos de exemplo para aula de hiperlink - imagem no ponteiro do mouse
</commit_message>
<xml_diff>
--- a/Ex11_Colisao/ver/PontosColisão.xlsx
+++ b/Ex11_Colisao/ver/PontosColisão.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="15315" windowHeight="5700" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="150" windowWidth="15315" windowHeight="5640"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -449,33 +449,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
@@ -483,67 +456,13 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -561,6 +480,87 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -865,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:AA31"/>
   <sheetViews>
-    <sheetView topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,13 +888,13 @@
       <c r="L3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="33" t="s">
+      <c r="M3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="47" t="s">
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="26" t="s">
         <v>1</v>
       </c>
       <c r="R3" s="10" t="s">
@@ -909,11 +909,11 @@
         <v>9</v>
       </c>
       <c r="L4" s="6"/>
-      <c r="M4" s="30"/>
+      <c r="M4" s="21"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
-      <c r="Q4" s="31"/>
+      <c r="Q4" s="22"/>
       <c r="T4" s="8" t="s">
         <v>8</v>
       </c>
@@ -938,11 +938,11 @@
         <v>17</v>
       </c>
       <c r="L5" s="6"/>
-      <c r="M5" s="30"/>
+      <c r="M5" s="21"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
-      <c r="Q5" s="31"/>
+      <c r="Q5" s="22"/>
       <c r="S5" s="9" t="s">
         <v>16</v>
       </c>
@@ -967,11 +967,11 @@
       <c r="I6" s="3"/>
       <c r="J6" s="4"/>
       <c r="L6" s="6"/>
-      <c r="M6" s="30"/>
+      <c r="M6" s="21"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
-      <c r="Q6" s="31"/>
+      <c r="Q6" s="22"/>
       <c r="S6" s="6"/>
       <c r="T6" s="2"/>
       <c r="U6" s="3"/>
@@ -987,15 +987,15 @@
       <c r="I7" s="3"/>
       <c r="J7" s="4"/>
       <c r="L7" s="6"/>
-      <c r="M7" s="49" t="s">
+      <c r="M7" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="N7" s="50"/>
+      <c r="N7" s="35"/>
       <c r="O7" s="3"/>
-      <c r="P7" s="38" t="s">
+      <c r="P7" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="Q7" s="39"/>
+      <c r="Q7" s="47"/>
       <c r="S7" s="6"/>
       <c r="T7" s="2"/>
       <c r="U7" s="3"/>
@@ -1013,13 +1013,13 @@
       <c r="L8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="51" t="s">
+      <c r="M8" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="N8" s="52"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="41"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="49"/>
       <c r="R8" s="10" t="s">
         <v>18</v>
       </c>
@@ -1035,10 +1035,10 @@
       <c r="F9" s="2"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="20" t="s">
+      <c r="I9" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="J9" s="21"/>
+      <c r="J9" s="53"/>
       <c r="M9" s="8" t="s">
         <v>15</v>
       </c>
@@ -1046,10 +1046,10 @@
         <v>14</v>
       </c>
       <c r="S9" s="6"/>
-      <c r="T9" s="24" t="s">
+      <c r="T9" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="U9" s="21"/>
+      <c r="U9" s="53"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
       <c r="X9" s="4"/>
@@ -1063,18 +1063,18 @@
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="23"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="55"/>
       <c r="K10" s="10" t="s">
         <v>18</v>
       </c>
       <c r="S10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="T10" s="25" t="s">
+      <c r="T10" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="U10" s="23"/>
+      <c r="U10" s="55"/>
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
       <c r="X10" s="14" t="s">
@@ -1144,15 +1144,15 @@
       <c r="C13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="34" t="s">
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="35" t="s">
+      <c r="H13" s="43" t="s">
         <v>1</v>
       </c>
       <c r="I13" s="10" t="s">
@@ -1170,13 +1170,13 @@
       <c r="U13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="V13" s="43" t="s">
+      <c r="V13" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="W13" s="44"/>
-      <c r="X13" s="29"/>
-      <c r="Y13" s="29"/>
-      <c r="Z13" s="47" t="s">
+      <c r="W13" s="39"/>
+      <c r="X13" s="20"/>
+      <c r="Y13" s="20"/>
+      <c r="Z13" s="26" t="s">
         <v>1</v>
       </c>
       <c r="AA13" s="10" t="s">
@@ -1185,11 +1185,11 @@
     </row>
     <row r="14" spans="3:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="6"/>
-      <c r="D14" s="30"/>
+      <c r="D14" s="21"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="37"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="45"/>
       <c r="K14" s="9"/>
       <c r="L14" s="19"/>
       <c r="M14" s="16"/>
@@ -1200,19 +1200,19 @@
       <c r="R14" s="18"/>
       <c r="S14" s="10"/>
       <c r="U14" s="6"/>
-      <c r="V14" s="45"/>
-      <c r="W14" s="46"/>
+      <c r="V14" s="40"/>
+      <c r="W14" s="41"/>
       <c r="X14" s="3"/>
       <c r="Y14" s="3"/>
-      <c r="Z14" s="31"/>
+      <c r="Z14" s="22"/>
     </row>
     <row r="15" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C15" s="6"/>
-      <c r="D15" s="30"/>
+      <c r="D15" s="21"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="31"/>
+      <c r="H15" s="22"/>
       <c r="K15" s="9"/>
       <c r="L15" s="19"/>
       <c r="M15" s="16"/>
@@ -1223,19 +1223,19 @@
       <c r="R15" s="18"/>
       <c r="S15" s="10"/>
       <c r="U15" s="6"/>
-      <c r="V15" s="30"/>
+      <c r="V15" s="21"/>
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
       <c r="Y15" s="3"/>
-      <c r="Z15" s="31"/>
+      <c r="Z15" s="22"/>
     </row>
     <row r="16" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C16" s="6"/>
-      <c r="D16" s="30"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="31"/>
+      <c r="H16" s="22"/>
       <c r="K16" s="9"/>
       <c r="L16" s="19"/>
       <c r="M16" s="16"/>
@@ -1246,21 +1246,21 @@
       <c r="R16" s="18"/>
       <c r="S16" s="10"/>
       <c r="U16" s="6"/>
-      <c r="V16" s="30"/>
+      <c r="V16" s="21"/>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
       <c r="Y16" s="3"/>
-      <c r="Z16" s="31"/>
+      <c r="Z16" s="22"/>
     </row>
     <row r="17" spans="3:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="6"/>
-      <c r="D17" s="30"/>
+      <c r="D17" s="21"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="38" t="s">
+      <c r="G17" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="H17" s="39"/>
+      <c r="H17" s="47"/>
       <c r="K17" s="9"/>
       <c r="L17" s="19"/>
       <c r="M17" s="16"/>
@@ -1271,25 +1271,25 @@
       <c r="R17" s="18"/>
       <c r="S17" s="10"/>
       <c r="U17" s="6"/>
-      <c r="V17" s="49" t="s">
+      <c r="V17" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="W17" s="50"/>
+      <c r="W17" s="35"/>
       <c r="X17" s="3"/>
       <c r="Y17" s="3"/>
-      <c r="Z17" s="31"/>
+      <c r="Z17" s="22"/>
     </row>
     <row r="18" spans="3:27" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="41"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="49"/>
       <c r="I18" s="10" t="s">
         <v>18</v>
       </c>
@@ -1305,13 +1305,13 @@
       <c r="U18" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="V18" s="51" t="s">
+      <c r="V18" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="W18" s="52"/>
-      <c r="X18" s="32"/>
-      <c r="Y18" s="32"/>
-      <c r="Z18" s="48" t="s">
+      <c r="W18" s="37"/>
+      <c r="X18" s="23"/>
+      <c r="Y18" s="23"/>
+      <c r="Z18" s="27" t="s">
         <v>2</v>
       </c>
       <c r="AA18" s="10" t="s">
@@ -1383,10 +1383,10 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="28" t="s">
+      <c r="I21" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="J21" s="27" t="s">
+      <c r="J21" s="59" t="s">
         <v>1</v>
       </c>
       <c r="K21" s="10" t="s">
@@ -1395,10 +1395,10 @@
       <c r="S21" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="T21" s="26" t="s">
+      <c r="T21" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="U21" s="27"/>
+      <c r="U21" s="59"/>
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="12" t="s">
@@ -1413,8 +1413,8 @@
       <c r="F22" s="2"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="23"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="55"/>
       <c r="M22" s="8" t="s">
         <v>8</v>
       </c>
@@ -1422,8 +1422,8 @@
         <v>9</v>
       </c>
       <c r="S22" s="6"/>
-      <c r="T22" s="25"/>
-      <c r="U22" s="23"/>
+      <c r="T22" s="57"/>
+      <c r="U22" s="55"/>
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
       <c r="X22" s="4"/>
@@ -1438,15 +1438,15 @@
       <c r="L23" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="M23" s="43" t="s">
+      <c r="M23" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="N23" s="44"/>
-      <c r="O23" s="29"/>
-      <c r="P23" s="53" t="s">
+      <c r="N23" s="39"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="Q23" s="35" t="s">
+      <c r="Q23" s="43" t="s">
         <v>1</v>
       </c>
       <c r="R23" s="10" t="s">
@@ -1467,11 +1467,11 @@
       <c r="I24" s="3"/>
       <c r="J24" s="4"/>
       <c r="L24" s="6"/>
-      <c r="M24" s="45"/>
-      <c r="N24" s="46"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="41"/>
       <c r="O24" s="3"/>
-      <c r="P24" s="54"/>
-      <c r="Q24" s="37"/>
+      <c r="P24" s="51"/>
+      <c r="Q24" s="45"/>
       <c r="S24" s="6"/>
       <c r="T24" s="2"/>
       <c r="U24" s="3"/>
@@ -1487,11 +1487,11 @@
       <c r="I25" s="3"/>
       <c r="J25" s="4"/>
       <c r="L25" s="6"/>
-      <c r="M25" s="30"/>
+      <c r="M25" s="21"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
-      <c r="Q25" s="31"/>
+      <c r="Q25" s="22"/>
       <c r="S25" s="6"/>
       <c r="T25" s="2"/>
       <c r="U25" s="3"/>
@@ -1516,11 +1516,11 @@
         <v>18</v>
       </c>
       <c r="L26" s="6"/>
-      <c r="M26" s="30"/>
+      <c r="M26" s="21"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
-      <c r="Q26" s="31"/>
+      <c r="Q26" s="22"/>
       <c r="S26" s="9" t="s">
         <v>19</v>
       </c>
@@ -1545,11 +1545,11 @@
         <v>14</v>
       </c>
       <c r="L27" s="6"/>
-      <c r="M27" s="30"/>
+      <c r="M27" s="21"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
-      <c r="Q27" s="31"/>
+      <c r="Q27" s="22"/>
       <c r="T27" s="8" t="s">
         <v>15</v>
       </c>
@@ -1561,13 +1561,13 @@
       <c r="L28" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M28" s="42" t="s">
+      <c r="M28" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="N28" s="32"/>
-      <c r="O28" s="32"/>
-      <c r="P28" s="32"/>
-      <c r="Q28" s="48" t="s">
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="27" t="s">
         <v>2</v>
       </c>
       <c r="R28" s="10" t="s">
@@ -1586,17 +1586,17 @@
     <row r="31" spans="3:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="V17:W18"/>
-    <mergeCell ref="V13:W14"/>
-    <mergeCell ref="G13:H14"/>
-    <mergeCell ref="P7:Q8"/>
-    <mergeCell ref="M7:N8"/>
     <mergeCell ref="P23:Q24"/>
     <mergeCell ref="M23:N24"/>
     <mergeCell ref="I9:J10"/>
     <mergeCell ref="T9:U10"/>
     <mergeCell ref="T21:U22"/>
     <mergeCell ref="I21:J22"/>
+    <mergeCell ref="V17:W18"/>
+    <mergeCell ref="V13:W14"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="P7:Q8"/>
+    <mergeCell ref="M7:N8"/>
     <mergeCell ref="G17:H18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1608,66 +1608,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.140625" style="55" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="28" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="55" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:4" ht="46.5" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="57" t="s">
+      <c r="C4" s="29"/>
+      <c r="D4" s="30" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="46.5" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B5" s="60"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="58"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="31"/>
     </row>
     <row r="6" spans="2:4" ht="46.5" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="57" t="s">
+      <c r="C6" s="29"/>
+      <c r="D6" s="30" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="46.5" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B7" s="60"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="58"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="31"/>
     </row>
     <row r="8" spans="2:4" ht="46.5" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="57" t="s">
+      <c r="C8" s="29"/>
+      <c r="D8" s="30" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="46.5" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B9" s="60"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="58"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="31"/>
     </row>
     <row r="10" spans="2:4" ht="46.5" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="57" t="s">
+      <c r="C10" s="29"/>
+      <c r="D10" s="30" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>